<commit_message>
feat: completed and documented case study for Course 1 Module 2
</commit_message>
<xml_diff>
--- a/excel-basics/formula/Revenue_Figures/Case Study - Revenue Figures.xlsx
+++ b/excel-basics/formula/Revenue_Figures/Case Study - Revenue Figures.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD90F13-FF26-43D7-AA31-6224F4477EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9908FFA2-75A4-4908-A58E-38A20FE6F4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B653257C-2690-4B6F-AF51-C145C2D6B17F}"/>
   </bookViews>
@@ -863,19 +863,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1195,8 +1195,8 @@
   <dimension ref="A1:Q202"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <pane ySplit="3" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L187" sqref="L187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,43 +1219,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="O1" t="s">
@@ -1266,19 +1266,19 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
       <c r="O2" t="s">
         <v>11</v>
       </c>
@@ -1288,19 +1288,19 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
       <c r="O3" t="s">
         <v>246</v>
       </c>
@@ -7252,6 +7252,11 @@
     <row r="202" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
     <mergeCell ref="M1:M3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
@@ -7260,11 +7265,6 @@
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="L1:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7277,7 +7277,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P75" sqref="P75"/>
+      <selection pane="bottomLeft" activeCell="G202" sqref="G202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7299,43 +7299,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="O1" t="s">
@@ -7346,19 +7346,19 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
       <c r="O2" t="s">
         <v>11</v>
       </c>
@@ -7368,23 +7368,23 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
       <c r="O3" t="s">
         <v>246</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="9">
         <f>M201/L201</f>
         <v>0.33333333333333315</v>
       </c>
@@ -16680,7 +16680,7 @@
         <v>523544.36874999997</v>
       </c>
       <c r="H197" s="7">
-        <f t="shared" ref="H197:H201" si="22">F197*$P$1</f>
+        <f t="shared" ref="H197:H200" si="22">F197*$P$1</f>
         <v>24943.75</v>
       </c>
       <c r="I197" s="7">
@@ -16688,7 +16688,7 @@
         <v>548488.11874999991</v>
       </c>
       <c r="J197" s="7">
-        <f t="shared" ref="J197:J201" si="24">(I197/F197)*1.5</f>
+        <f t="shared" ref="J197:J200" si="24">(I197/F197)*1.5</f>
         <v>164.91749999999996</v>
       </c>
       <c r="K197" s="3">
@@ -16696,7 +16696,7 @@
         <v>4988.75</v>
       </c>
       <c r="L197" s="1">
-        <f t="shared" ref="L197:L201" si="26">J197*K197</f>
+        <f t="shared" ref="L197:L200" si="26">J197*K197</f>
         <v>822732.17812499986</v>
       </c>
       <c r="M197" s="7">
@@ -16850,11 +16850,11 @@
     </row>
     <row r="201" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G201" s="5">
-        <f t="shared" ref="G201:M201" si="28">SUM(G4:G200)</f>
+        <f>SUM(G4:G200)</f>
         <v>70764990.998125017</v>
       </c>
       <c r="H201" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="G201:L201" si="28">SUM(H4:H200)</f>
         <v>4301328.75</v>
       </c>
       <c r="I201" s="5">
@@ -16881,6 +16881,12 @@
     <row r="202" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="M1:M3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
@@ -16888,12 +16894,6 @@
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="K1:K3"/>
     <mergeCell ref="L1:L3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16901,26 +16901,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EAC3B332A2FD04E918F9FD72E2B30AC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5791f7a1e5ce60c682c7fd472657cfed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aed4346-8012-4133-9837-e496d0f5c99a" xmlns:ns3="15179a99-4cef-4bac-ab20-a4c03d7ec5db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4db72e02b896ab7bb9242ff846c9720" ns2:_="" ns3:_="">
     <xsd:import namespace="2aed4346-8012-4133-9837-e496d0f5c99a"/>
@@ -17137,26 +17117,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD4C417B-C4D3-4673-B18D-F0AA474BC7ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
-    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{538C5C99-AEA9-45C8-8A4A-73C68FBF2871}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B840969E-CDB0-426E-91F0-A655AB06EC6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17173,4 +17154,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{538C5C99-AEA9-45C8-8A4A-73C68FBF2871}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD4C417B-C4D3-4673-B18D-F0AA474BC7ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
+    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>